<commit_message>
added code for adjusting mass error above the current lockmass range with a linear fit
</commit_message>
<xml_diff>
--- a/products analysis/fatacidref source.xlsx
+++ b/products analysis/fatacidref source.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skutarna\Documents\MSc 2\NTA\TargetDecoy\products analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Steven\Target Decoy\products analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{32000E3F-AB28-4DE8-ACC8-9FC29AFFAFA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D97786E-1A54-4E30-B505-D31CEE2387F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref Find" sheetId="1" r:id="rId1"/>
     <sheet name="Calibration Testing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>Sample 100 m/z</t>
   </si>
@@ -92,12 +100,6 @@
     <t>Ref m/z</t>
   </si>
   <si>
-    <t>In Raw Data</t>
-  </si>
-  <si>
-    <t>In Cal Data</t>
-  </si>
-  <si>
     <t>C14H21O7</t>
   </si>
   <si>
@@ -130,11 +132,23 @@
   <si>
     <t>Theoretical m/z +e</t>
   </si>
+  <si>
+    <t>Raw Data</t>
+  </si>
+  <si>
+    <t>Cal Data original code</t>
+  </si>
+  <si>
+    <t>Cal Data with higher lockmasses and 1/x fit option</t>
+  </si>
+  <si>
+    <t>Cal Data as above plus high range linear fit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1160,6 +1174,16 @@
               <a:t>Calibration Effectiveness - Reference Compounds</a:t>
             </a:r>
           </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t>Sample 100</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -1206,14 +1230,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>In Raw Data</c:v>
+                  <c:v>Raw Data</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1269,37 +1295,37 @@
                 <c:pt idx="9">
                   <c:v>283.26380569999998</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>317.09088000000003</c:v>
+                </c:pt>
                 <c:pt idx="11">
-                  <c:v>317.09088000000003</c:v>
+                  <c:v>325.1837883</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>325.1837883</c:v>
+                  <c:v>326.1818007</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>326.1818007</c:v>
+                  <c:v>339.19934160000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>339.19934160000003</c:v>
+                  <c:v>361.11690320000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>361.11690320000002</c:v>
+                  <c:v>369.2126993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>369.2126993</c:v>
+                  <c:v>381.23106949999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>381.23106949999999</c:v>
+                  <c:v>401.08731289999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>401.08731289999997</c:v>
+                  <c:v>415.21826090000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>415.21826090000002</c:v>
+                  <c:v>459.24449390000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>459.24449390000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>503.27086539999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -1341,37 +1367,37 @@
                 <c:pt idx="9">
                   <c:v>-1.5861514189775325</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.95240743710270614</c:v>
+                </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.95240743710270614</c:v>
+                  <c:v>-1.5489678079759963</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.5489678079759963</c:v>
+                  <c:v>-0.74590249353373195</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.74590249353373195</c:v>
+                  <c:v>-1.7700474722938702</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.7700474722938702</c:v>
+                  <c:v>-1.3674223509047818</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.3674223509047818</c:v>
+                  <c:v>-0.84151964200827356</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.84151964200827356</c:v>
+                  <c:v>-1.4885962887395039</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-1.4885962887395039</c:v>
+                  <c:v>-1.2393794765745578</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.2393794765745578</c:v>
+                  <c:v>-0.5517577022061475</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.5517577022061475</c:v>
+                  <c:v>-0.45966779289160986</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.45966779289160986</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>-0.10849027398319072</c:v>
                 </c:pt>
               </c:numCache>
@@ -1393,14 +1419,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>In Cal Data</c:v>
+                  <c:v>Cal Data original code</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1456,34 +1484,34 @@
                 <c:pt idx="9">
                   <c:v>283.26408177341</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>317.09116637818499</c:v>
+                </c:pt>
                 <c:pt idx="11">
-                  <c:v>317.09116637818499</c:v>
+                  <c:v>325.18420587249199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>325.18420587249199</c:v>
+                  <c:v>326.18212407633501</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>326.18212407633501</c:v>
+                  <c:v>339.199730777789</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>339.199730777789</c:v>
+                  <c:v>369.21315026200301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>381.23147716725299</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>369.21315026200301</c:v>
+                  <c:v>401.087666059951</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>381.23147716725299</c:v>
+                  <c:v>415.21875815311699</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>401.087666059951</c:v>
+                  <c:v>459.244950692261</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>415.21875815311699</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>459.244950692261</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>503.271450915294</c:v>
                 </c:pt>
               </c:numCache>
@@ -1525,34 +1553,34 @@
                 <c:pt idx="9">
                   <c:v>-0.61153706101460537</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.9266002640152393E-2</c:v>
+                </c:pt>
                 <c:pt idx="11">
-                  <c:v>-4.9266002640152393E-2</c:v>
+                  <c:v>-0.26485752880155006</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.26485752880155006</c:v>
+                  <c:v>0.24549584051469514</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24549584051469514</c:v>
+                  <c:v>-0.62270709634873411</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.62270709634873411</c:v>
+                  <c:v>0.37989453030072867</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.41925362817627687</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.37989453030072867</c:v>
+                  <c:v>-0.35887415522742749</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.41925362817627687</c:v>
+                  <c:v>0.64581208081476571</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.35887415522742749</c:v>
+                  <c:v>0.53499203882234259</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.64581208081476571</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.53499203882234259</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>1.0549294086119116</c:v>
                 </c:pt>
               </c:numCache>
@@ -1712,6 +1740,344 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-1E49-4CEC-954C-E64FB4F1CF07}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calibration Testing'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cal Data with higher lockmasses and 1/x fit option</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calibration Testing'!$L$2:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>129.01933500000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.050635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>171.01214200000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>171.10267000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>187.09758500000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>189.07685000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>201.113235</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>233.10306500000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>255.232955</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>283.26425499999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>325.18429199999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>339.19994199999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>361.11739699999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>369.21301</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>381.23163699999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>401.08780999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>415.21848999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>459.24470499999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calibration Testing'!$N$2:$N$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>-0.12184534996883156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15498929040151532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6547126007468727E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.8939041739922006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-8.7672638872092465E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.5593389707079965E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.655174312743072E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0898667435954345E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.71615024793915361</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12029327523814945</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.17214661766696263</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4365570334750106E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-8.1212589656592366E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.42466237310187066</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.21816108616792204</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0034051114798599E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68655702212631575</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.82283402930289495</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3B50-4486-B0BC-DB857FFEF947}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calibration Testing'!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cal Data as above plus high range linear fit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calibration Testing'!$P$2:$P$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>129.01933500000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.050635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>171.01214200000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>171.10267000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>187.09758500000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>189.07685000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>201.113235</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>233.10306500000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>255.232955</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>283.26425499999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>325.18429199999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>339.19994199999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>361.11739699999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>369.21301</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>381.23163699999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>401.08780999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>415.21848999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>459.24470499999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calibration Testing'!$R$2:$R$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>-0.12184534996883156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15498929040151532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6547126007468727E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.8939041739922006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-8.7672638872092465E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.5593389707079965E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.655174312743072E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0898667435954345E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.71615024793915361</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12029327523814945</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2801381220253682E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.16158187004241817</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.33616264964346831</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.10628512790940244</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.48785246011252115</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.50018833276988062</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8195252397560935E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.19393792016716049</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3B50-4486-B0BC-DB857FFEF947}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1988,11 +2354,11 @@
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="4"/>
+        <c:idx val="6"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="5"/>
+        <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -3227,15 +3593,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>170039</xdr:colOff>
+      <xdr:colOff>265286</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>40922</xdr:rowOff>
+      <xdr:rowOff>40923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>56445</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>119944</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>444498</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3267,12 +3633,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.79678</cdr:x>
-      <cdr:y>0.21403</cdr:y>
+      <cdr:x>0.74804</cdr:x>
+      <cdr:y>0.2282</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.92565</cdr:x>
-      <cdr:y>0.29996</cdr:y>
+      <cdr:x>0.87691</cdr:x>
+      <cdr:y>0.31413</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3287,8 +3653,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4083050" y="838200"/>
-          <a:ext cx="660400" cy="336550"/>
+          <a:off x="8771247" y="1533923"/>
+          <a:ext cx="1511081" cy="577606"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3605,21 +3971,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3642,7 +4008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>129.0181</v>
       </c>
@@ -3666,7 +4032,7 @@
         <v>129.01933500000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>145.04949999999999</v>
       </c>
@@ -3690,7 +4056,7 @@
         <v>145.050635</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>171.0111</v>
       </c>
@@ -3714,7 +4080,7 @@
         <v>171.01214200000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>171.10159999999999</v>
       </c>
@@ -3738,7 +4104,7 @@
         <v>171.10267000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>187.09649999999999</v>
       </c>
@@ -3762,7 +4128,7 @@
         <v>187.09758500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>189.07589999999999</v>
       </c>
@@ -3786,7 +4152,7 @@
         <v>189.07685000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>201.1123</v>
       </c>
@@ -3810,7 +4176,7 @@
         <v>201.113235</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>233.10239999999999</v>
       </c>
@@ -3834,7 +4200,7 @@
         <v>233.10306500000002</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>255.23249999999999</v>
       </c>
@@ -3858,7 +4224,7 @@
         <v>255.232955</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>283.2638</v>
       </c>
@@ -3882,7 +4248,7 @@
         <v>283.26425499999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>301.12889999999999</v>
       </c>
@@ -3890,7 +4256,7 @@
         <v>3670000</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>-1.2490000000000001</v>
@@ -3906,7 +4272,7 @@
         <v>301.12927999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>317.09100000000001</v>
       </c>
@@ -3914,7 +4280,7 @@
         <v>206000</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>-0.55500000000000005</v>
@@ -3930,7 +4296,7 @@
         <v>317.091182</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>325.18400000000003</v>
       </c>
@@ -3938,7 +4304,7 @@
         <v>87800000</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>-0.88800000000000001</v>
@@ -3954,7 +4320,7 @@
         <v>325.18429199999997</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>326.18180000000001</v>
       </c>
@@ -3962,7 +4328,7 @@
         <v>699000</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>-0.73599999999999999</v>
@@ -3978,7 +4344,7 @@
         <v>326.18204399999996</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>339.19959999999998</v>
       </c>
@@ -3986,7 +4352,7 @@
         <v>42000000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16">
         <v>-0.999</v>
@@ -4002,7 +4368,7 @@
         <v>339.19994199999996</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>361.11689999999999</v>
       </c>
@@ -4010,7 +4376,7 @@
         <v>620000</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>-1.359</v>
@@ -4026,7 +4392,7 @@
         <v>361.11739699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>369.21269999999998</v>
       </c>
@@ -4034,7 +4400,7 @@
         <v>21600000</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>-0.82799999999999996</v>
@@ -4050,7 +4416,7 @@
         <v>369.21301</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>381.2312</v>
       </c>
@@ -4058,7 +4424,7 @@
         <v>3630000</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>-1.135</v>
@@ -4074,7 +4440,7 @@
         <v>381.23163699999998</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>401.0874</v>
       </c>
@@ -4082,7 +4448,7 @@
         <v>8780000</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>-1.0109999999999999</v>
@@ -4098,7 +4464,7 @@
         <v>401.08780999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>415.2183</v>
       </c>
@@ -4122,7 +4488,7 @@
         <v>415.21848999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>459.24439999999998</v>
       </c>
@@ -4146,7 +4512,7 @@
         <v>459.24470499999995</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>503.27080000000001</v>
       </c>
@@ -4170,7 +4536,7 @@
         <v>503.27091999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>547.29700000000003</v>
       </c>
@@ -4194,7 +4560,7 @@
         <v>547.29713500000003</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>591.32360000000006</v>
       </c>
@@ -4230,43 +4596,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="9" max="9" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>129.01933500000001</v>
       </c>
@@ -4290,8 +4675,28 @@
       <c r="J2" t="s">
         <v>7</v>
       </c>
+      <c r="L2">
+        <v>129.01933500000001</v>
+      </c>
+      <c r="M2">
+        <v>129.01931927959399</v>
+      </c>
+      <c r="N2">
+        <f>(M2-L2)/L2*10^6</f>
+        <v>-0.12184534996883156</v>
+      </c>
+      <c r="P2">
+        <v>129.01933500000001</v>
+      </c>
+      <c r="Q2">
+        <v>129.01931927959399</v>
+      </c>
+      <c r="R2">
+        <f>(Q2-P2)/P2*10^6</f>
+        <v>-0.12184534996883156</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>145.050635</v>
       </c>
@@ -4315,8 +4720,28 @@
       <c r="J3" t="s">
         <v>6</v>
       </c>
+      <c r="L3">
+        <v>145.050635</v>
+      </c>
+      <c r="M3">
+        <v>145.05065748129499</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N20" si="2">(M3-L3)/L3*10^6</f>
+        <v>0.15498929040151532</v>
+      </c>
+      <c r="P3">
+        <v>145.050635</v>
+      </c>
+      <c r="Q3">
+        <v>145.05065748129499</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R25" si="3">(Q3-P3)/P3*10^6</f>
+        <v>0.15498929040151532</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>171.01214200000001</v>
       </c>
@@ -4340,8 +4765,28 @@
       <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L4" s="2">
+        <v>171.01214200000001</v>
+      </c>
+      <c r="M4">
+        <v>171.01215509048799</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>7.6547126007468727E-2</v>
+      </c>
+      <c r="P4" s="2">
+        <v>171.01214200000001</v>
+      </c>
+      <c r="Q4">
+        <v>171.01215509048799</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="3"/>
+        <v>7.6547126007468727E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>171.10267000000002</v>
       </c>
@@ -4365,8 +4810,28 @@
       <c r="J5" t="s">
         <v>9</v>
       </c>
+      <c r="L5">
+        <v>171.10267000000002</v>
+      </c>
+      <c r="M5">
+        <v>171.10266333742601</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>-3.8939041739922006E-2</v>
+      </c>
+      <c r="P5">
+        <v>171.10267000000002</v>
+      </c>
+      <c r="Q5">
+        <v>171.10266333742601</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="3"/>
+        <v>-3.8939041739922006E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>187.09758500000001</v>
       </c>
@@ -4390,8 +4855,28 @@
       <c r="J6" t="s">
         <v>11</v>
       </c>
+      <c r="L6">
+        <v>187.09758500000001</v>
+      </c>
+      <c r="M6">
+        <v>187.09756859666101</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>-8.7672638872092465E-2</v>
+      </c>
+      <c r="P6">
+        <v>187.09758500000001</v>
+      </c>
+      <c r="Q6">
+        <v>187.09756859666101</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>-8.7672638872092465E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>189.07685000000001</v>
       </c>
@@ -4415,8 +4900,28 @@
       <c r="J7" t="s">
         <v>14</v>
       </c>
+      <c r="L7">
+        <v>189.07685000000001</v>
+      </c>
+      <c r="M7">
+        <v>189.076831925503</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>-9.5593389707079965E-2</v>
+      </c>
+      <c r="P7">
+        <v>189.07685000000001</v>
+      </c>
+      <c r="Q7">
+        <v>189.076831925503</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>-9.5593389707079965E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>201.113235</v>
       </c>
@@ -4440,8 +4945,28 @@
       <c r="J8" t="s">
         <v>12</v>
       </c>
+      <c r="L8">
+        <v>201.113235</v>
+      </c>
+      <c r="M8">
+        <v>201.113223626696</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>-5.655174312743072E-2</v>
+      </c>
+      <c r="P8">
+        <v>201.113235</v>
+      </c>
+      <c r="Q8">
+        <v>201.113223626696</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>-5.655174312743072E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>233.10306500000002</v>
       </c>
@@ -4465,8 +4990,28 @@
       <c r="J9" t="s">
         <v>15</v>
       </c>
+      <c r="L9">
+        <v>233.10306500000002</v>
+      </c>
+      <c r="M9">
+        <v>233.103086188758</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>9.0898667435954345E-2</v>
+      </c>
+      <c r="P9">
+        <v>233.10306500000002</v>
+      </c>
+      <c r="Q9">
+        <v>233.103086188758</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>9.0898667435954345E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>255.232955</v>
       </c>
@@ -4490,8 +5035,28 @@
       <c r="J10" t="s">
         <v>13</v>
       </c>
+      <c r="L10">
+        <v>255.232955</v>
+      </c>
+      <c r="M10">
+        <v>255.23313778514401</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>0.71615024793915361</v>
+      </c>
+      <c r="P10">
+        <v>255.232955</v>
+      </c>
+      <c r="Q10">
+        <v>255.23313778514401</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>0.71615024793915361</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>283.26425499999999</v>
       </c>
@@ -4515,203 +5080,404 @@
       <c r="J11" t="s">
         <v>16</v>
       </c>
+      <c r="L11">
+        <v>283.26425499999999</v>
+      </c>
+      <c r="M11">
+        <v>283.26428907478498</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>0.12029327523814945</v>
+      </c>
+      <c r="P11">
+        <v>283.26425499999999</v>
+      </c>
+      <c r="Q11">
+        <v>283.26428907478498</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>0.12029327523814945</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>301.12927999999999</v>
       </c>
+      <c r="C12">
+        <v>317.09088000000003</v>
+      </c>
+      <c r="D12">
+        <f>(C12-A13)/A13*10^6</f>
+        <v>-0.95240743710270614</v>
+      </c>
+      <c r="F12">
+        <v>317.09116637818499</v>
+      </c>
+      <c r="G12">
+        <f>(F12-A13)/A13*10^6</f>
+        <v>-4.9266002640152393E-2</v>
+      </c>
       <c r="I12">
         <v>317.091182</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="L12" s="2">
+        <v>325.18429199999997</v>
+      </c>
+      <c r="M12">
+        <v>325.18423602062398</v>
+      </c>
+      <c r="N12">
+        <f>(M12-L12)/L12*10^6</f>
+        <v>-0.17214661766696263</v>
+      </c>
+      <c r="P12" s="2">
+        <v>325.18429199999997</v>
+      </c>
+      <c r="Q12">
+        <v>325.18429941465098</v>
+      </c>
+      <c r="R12">
+        <f>(Q12-P12)/P12*10^6</f>
+        <v>2.2801381220253682E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>317.091182</v>
       </c>
       <c r="C13">
-        <v>317.09088000000003</v>
+        <v>325.1837883</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>-0.95240743710270614</v>
+        <f>(C13-A14)/A14*10^6</f>
+        <v>-1.5489678079759963</v>
       </c>
       <c r="F13">
-        <v>317.09116637818499</v>
+        <v>325.18420587249199</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G20" si="2">(F13-A13)/A13*10^6</f>
-        <v>-4.9266002640152393E-2</v>
+        <f>(F13-A14)/A14*10^6</f>
+        <v>-0.26485752880155006</v>
       </c>
       <c r="I13">
         <v>325.18429199999997</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="L13" s="2">
+        <v>339.19994199999996</v>
+      </c>
+      <c r="M13">
+        <v>339.19995026480001</v>
+      </c>
+      <c r="N13">
+        <f>(M13-L13)/L13*10^6</f>
+        <v>2.4365570334750106E-2</v>
+      </c>
+      <c r="P13" s="2">
+        <v>339.19994199999996</v>
+      </c>
+      <c r="Q13">
+        <v>339.19988719143902</v>
+      </c>
+      <c r="R13">
+        <f>(Q13-P13)/P13*10^6</f>
+        <v>-0.16158187004241817</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>325.18429199999997</v>
       </c>
       <c r="C14">
-        <v>325.1837883</v>
+        <v>326.1818007</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>-1.5489678079759963</v>
+        <f>(C14-A15)/A15*10^6</f>
+        <v>-0.74590249353373195</v>
       </c>
       <c r="F14">
-        <v>325.18420587249199</v>
+        <v>326.18212407633501</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
-        <v>-0.26485752880155006</v>
+        <f>(F14-A15)/A15*10^6</f>
+        <v>0.24549584051469514</v>
       </c>
       <c r="I14">
         <v>326.18204399999996</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="L14" s="2">
+        <v>361.11739699999998</v>
+      </c>
+      <c r="M14">
+        <v>361.117367672721</v>
+      </c>
+      <c r="N14">
+        <f>(M14-L14)/L14*10^6</f>
+        <v>-8.1212589656592366E-2</v>
+      </c>
+      <c r="P14" s="2">
+        <v>361.11739699999998</v>
+      </c>
+      <c r="Q14">
+        <v>361.11727560581897</v>
+      </c>
+      <c r="R14">
+        <f>(Q14-P14)/P14*10^6</f>
+        <v>-0.33616264964346831</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>326.18204399999996</v>
       </c>
       <c r="C15">
-        <v>326.1818007</v>
+        <v>339.19934160000003</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>-0.74590249353373195</v>
+        <f>(C15-A16)/A16*10^6</f>
+        <v>-1.7700474722938702</v>
       </c>
       <c r="F15">
-        <v>326.18212407633501</v>
+        <v>339.199730777789</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
-        <v>0.24549584051469514</v>
+        <f>(F15-A16)/A16*10^6</f>
+        <v>-0.62270709634873411</v>
       </c>
       <c r="I15">
         <v>339.19994199999996</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="L15">
+        <v>369.21301</v>
+      </c>
+      <c r="M15">
+        <v>369.213166790873</v>
+      </c>
+      <c r="N15">
+        <f>(M15-L15)/L15*10^6</f>
+        <v>0.42466237310187066</v>
+      </c>
+      <c r="P15">
+        <v>369.21301</v>
+      </c>
+      <c r="Q15">
+        <v>369.21304924185199</v>
+      </c>
+      <c r="R15">
+        <f>(Q15-P15)/P15*10^6</f>
+        <v>0.10628512790940244</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>339.19994199999996</v>
       </c>
       <c r="C16">
-        <v>339.19934160000003</v>
+        <v>361.11690320000002</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>-1.7700474722938702</v>
+        <f>(C16-A17)/A17*10^6</f>
+        <v>-1.3674223509047818</v>
       </c>
       <c r="F16">
-        <v>339.199730777789</v>
+        <v>369.21315026200301</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
-        <v>-0.62270709634873411</v>
+        <f>(F16-A18)/A18*10^6</f>
+        <v>0.37989453030072867</v>
       </c>
       <c r="I16">
         <v>361.11739699999998</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="L16" s="2">
+        <v>381.23163699999998</v>
+      </c>
+      <c r="M16">
+        <v>381.23172016990799</v>
+      </c>
+      <c r="N16">
+        <f>(M16-L16)/L16*10^6</f>
+        <v>0.21816108616792204</v>
+      </c>
+      <c r="P16" s="2">
+        <v>381.23163699999998</v>
+      </c>
+      <c r="Q16">
+        <v>381.23145101520799</v>
+      </c>
+      <c r="R16">
+        <f>(Q16-P16)/P16*10^6</f>
+        <v>-0.48785246011252115</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>361.11739699999998</v>
       </c>
       <c r="C17">
-        <v>361.11690320000002</v>
+        <v>369.2126993</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>-1.3674223509047818</v>
+        <f>(C17-A18)/A18*10^6</f>
+        <v>-0.84151964200827356</v>
+      </c>
+      <c r="F17">
+        <v>381.23147716725299</v>
+      </c>
+      <c r="G17">
+        <f>(F17-A19)/A19*10^6</f>
+        <v>-0.41925362817627687</v>
       </c>
       <c r="I17">
         <v>369.21301</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="L17">
+        <v>401.08780999999999</v>
+      </c>
+      <c r="M17">
+        <v>401.08781160571698</v>
+      </c>
+      <c r="N17">
+        <f>(M17-L17)/L17*10^6</f>
+        <v>4.0034051114798599E-3</v>
+      </c>
+      <c r="P17">
+        <v>401.08780999999999</v>
+      </c>
+      <c r="Q17">
+        <v>401.08760938055701</v>
+      </c>
+      <c r="R17">
+        <f>(Q17-P17)/P17*10^6</f>
+        <v>-0.50018833276988062</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>369.21301</v>
       </c>
       <c r="C18">
-        <v>369.2126993</v>
+        <v>381.23106949999999</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>-0.84151964200827356</v>
+        <f>(C18-A19)/A19*10^6</f>
+        <v>-1.4885962887395039</v>
       </c>
       <c r="F18">
-        <v>369.21315026200301</v>
+        <v>401.087666059951</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
-        <v>0.37989453030072867</v>
+        <f>(F18-A20)/A20*10^6</f>
+        <v>-0.35887415522742749</v>
       </c>
       <c r="I18">
         <v>381.23163699999998</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="L18">
+        <v>415.21848999999997</v>
+      </c>
+      <c r="M18">
+        <v>415.21877507117</v>
+      </c>
+      <c r="N18">
+        <f>(M18-L18)/L18*10^6</f>
+        <v>0.68655702212631575</v>
+      </c>
+      <c r="P18">
+        <v>415.21848999999997</v>
+      </c>
+      <c r="Q18">
+        <v>415.218505859375</v>
+      </c>
+      <c r="R18">
+        <f>(Q18-P18)/P18*10^6</f>
+        <v>3.8195252397560935E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>381.23163699999998</v>
       </c>
       <c r="C19">
-        <v>381.23106949999999</v>
+        <v>401.08731289999997</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>-1.4885962887395039</v>
+        <f>(C19-A20)/A20*10^6</f>
+        <v>-1.2393794765745578</v>
       </c>
       <c r="F19">
-        <v>381.23147716725299</v>
+        <v>415.21875815311699</v>
       </c>
       <c r="G19">
-        <f t="shared" si="2"/>
-        <v>-0.41925362817627687</v>
+        <f>(F19-A21)/A21*10^6</f>
+        <v>0.64581208081476571</v>
       </c>
       <c r="I19">
         <v>401.08780999999999</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="L19">
+        <v>459.24470499999995</v>
+      </c>
+      <c r="M19">
+        <v>459.245082882171</v>
+      </c>
+      <c r="N19">
+        <f>(M19-L19)/L19*10^6</f>
+        <v>0.82283402930289495</v>
+      </c>
+      <c r="P19">
+        <v>459.24470499999995</v>
+      </c>
+      <c r="Q19">
+        <v>459.24461593503702</v>
+      </c>
+      <c r="R19">
+        <f>(Q19-P19)/P19*10^6</f>
+        <v>-0.19393792016716049</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>401.08780999999999</v>
       </c>
       <c r="C20">
-        <v>401.08731289999997</v>
+        <v>415.21826090000002</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>-1.2393794765745578</v>
+        <f>(C20-A21)/A21*10^6</f>
+        <v>-0.5517577022061475</v>
       </c>
       <c r="F20">
-        <v>401.087666059951</v>
+        <v>459.244950692261</v>
       </c>
       <c r="G20">
-        <f t="shared" si="2"/>
-        <v>-0.35887415522742749</v>
+        <f>(F20-A22)/A22*10^6</f>
+        <v>0.53499203882234259</v>
       </c>
       <c r="I20">
         <v>415.21848999999997</v>
@@ -4720,23 +5486,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>415.21848999999997</v>
       </c>
       <c r="C21">
-        <v>415.21826090000002</v>
+        <v>459.24449390000001</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>-0.5517577022061475</v>
+        <f>(C21-A22)/A22*10^6</f>
+        <v>-0.45966779289160986</v>
       </c>
       <c r="F21">
-        <v>415.21875815311699</v>
+        <v>503.271450915294</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
-        <v>0.64581208081476571</v>
+        <f>(F21-A23)/A23*10^6</f>
+        <v>1.0549294086119116</v>
       </c>
       <c r="I21">
         <v>459.24470499999995</v>
@@ -4745,23 +5511,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>459.24470499999995</v>
       </c>
       <c r="C22">
-        <v>459.24449390000001</v>
+        <v>503.27086539999999</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>-0.45966779289160986</v>
-      </c>
-      <c r="F22">
-        <v>459.244950692261</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="1"/>
-        <v>0.53499203882234259</v>
+        <f>(C22-A23)/A23*10^6</f>
+        <v>-0.10849027398319072</v>
       </c>
       <c r="I22">
         <v>503.27091999999999</v>
@@ -4770,36 +5529,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>503.27091999999999</v>
       </c>
-      <c r="C23">
-        <v>503.27086539999999</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>-0.10849027398319072</v>
-      </c>
-      <c r="F23">
-        <v>503.271450915294</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="1"/>
-        <v>1.0549294086119116</v>
-      </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>547.29713500000003</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>591.32335</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>0</v>
       </c>
@@ -4813,7 +5558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>550</v>
       </c>

</xml_diff>